<commit_message>
Added task BSLists -> 'Снимок БГ.txt'
</commit_message>
<xml_diff>
--- a/Списки.xlsx
+++ b/Списки.xlsx
@@ -7676,7 +7676,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7854,7 +7854,7 @@
       </c>
     </row>
     <row r="22" s="26" customFormat="true" ht="217.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="24" t="s">
         <v>226</v>
       </c>
       <c r="B22" s="35" t="s">

</xml_diff>

<commit_message>
fix(bs_lists): fix function for 'Существительные м. р.txt'
</commit_message>
<xml_diff>
--- a/Списки.xlsx
+++ b/Списки.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ТВ-ВО\а также\ТЕКСТ ПРОГРАММА\+ генератор списков\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1C1064-88FB-4E08-BF25-5000E8722D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EB195A-E88C-4936-A6DF-ABCE38095FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1017,34 +1017,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Найти в БС строки с ЗС групп, идентификатор которых содержит </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.С </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, и в ЗС имеется хотя бы 1 дефис.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Найти в БС строки с ЗС групп с идентификатором </t>
     </r>
     <r>
@@ -1092,34 +1064,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Найти в БС строки с ЗС групп, идентификатор которых содержит </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.С </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, и в ЗС имеется более 1 дефиса.</t>
     </r>
   </si>
   <si>
@@ -6070,6 +6014,347 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve">, и в спец. информации в составе шаблона ед. ч.:                                                                                                                           а. имеется указатель муж. рода </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">м </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>и отсутствует дефис</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(кроме ЗС групп с идентификатором</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> .СеИ-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">или                                                                                                                                                                                                                                                                                                     б. имеется указатель муж. рода с индикатором "!" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>м!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> и отсутствует дефис (кроме ЗС групп с идентификатором </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.СеИ-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) или                                                                                                                                                                                                                                                                                                                            в. имеются указатель муж. рода </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>м</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> и указатель муж. рода с предшествующим дефисом </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-м</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>м</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>…</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-м</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">…) или                                                                                                                                                                                                                    г. имеются указатель муж. рода с индикатором "!" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>м!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> и указатель муж. рода с индикатором "!" с предшествующим дефисом </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-м!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>м!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>…</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-м!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>…).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Найти в БС строки с ЗС групп, идентификатор которых содержит </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.С </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>и не содержит символ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">, и в спец. информации в составе шаблона ед. ч.:                                                                                                                                                                                  а. имеется указатель жен. рода </t>
     </r>
     <r>
@@ -6091,7 +6376,28 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>и отсутствует дефис</t>
+      <t xml:space="preserve">и отсутствует дефис (кроме ЗС групп с идентификатором </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.СеИ-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
     </r>
     <r>
       <rPr>
@@ -6112,7 +6418,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">или                                                                                                                                                                                                                                                                                              б. имеется указатель жен. рода </t>
+      <t xml:space="preserve">или                                                                                                                                                                                                                                                                                              б. имеется указатель жен. рода с индикатором "!" </t>
     </r>
     <r>
       <rPr>
@@ -6133,7 +6439,28 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> и отсутствует дефис или                                                                                                                                                                                                                                                                                                     в. имеются указатель жен. рода </t>
+      <t xml:space="preserve"> и отсутствует дефис (кроме ЗС групп с идентификатором </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.СеИ-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) или                                                                                                                                                                                                                                                                                                     в. имеются указатель жен. рода </t>
     </r>
     <r>
       <rPr>
@@ -6217,6 +6544,90 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve">…) или                                                                                                                                                                                                                 г. имеются указатель жен. рода с индикатором "!" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ж! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">и указатель жен. рода с индикатором "!" с предшествующим дефисом </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-ж!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ж!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>…</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-ж!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>…).</t>
     </r>
   </si>
@@ -6264,28 +6675,49 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">, и в спец. информации в составе шаблона ед. ч.:                                                                                                                           а. имеется указатель муж. рода </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">м </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>и отсутствует дефис</t>
+      <t xml:space="preserve">, и в спец. информации в составе шаблона ед. ч.:                                                                                                                                                                             а. имеется указатель ср. рода </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">с </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">и отсутствует дефис (кроме ЗС групп с идентификатором </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.СеИ-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
     </r>
     <r>
       <rPr>
@@ -6306,60 +6738,81 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">или                                                                                                                                                                                                                                                                                                     б. имеется указатель муж. рода </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>м!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> и отсутствует дефис или                                                                                                                                                                                                                                                                                                                            в. имеются указатель муж. рода </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>м</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> и указатель муж. рода с предшествующим дефисом </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-м</t>
+      <t xml:space="preserve">или                                                                                                                                                                                                                                                                                                    б. имеется указатель ср. рода с индикатором "!" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>с!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> и отсутствует дефис (кроме ЗС групп с идентификатором </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.СеИ-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) или                                                                                                                                                                                                                                                                                                                    в. имеются указатель ср. рода </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>с</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> и указатель ср. рода с предшествующим дефисом </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-с</t>
     </r>
     <r>
       <rPr>
@@ -6380,7 +6833,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>м</t>
+      <t>с</t>
     </r>
     <r>
       <rPr>
@@ -6401,7 +6854,91 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>-м</t>
+      <t>-с</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">…) или                                                                                                                                                                                                               г. имеются указатель ср. рода с индикатором "!" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>с!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> и указатель ср. рода с индикатором "!" с предшествующим дефисом </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-с!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>с!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>…</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-с!</t>
     </r>
     <r>
       <rPr>
@@ -6422,6 +6959,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="204"/>
@@ -6432,6 +6970,7 @@
     <r>
       <rPr>
         <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="204"/>
@@ -6443,6 +6982,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="204"/>
@@ -6453,159 +6993,64 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, и в спец. информации в составе шаблона ед. ч.:                                                                                                                                                                             а. имеется указатель ср. рода </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">с </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>и отсутствует дефис</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">или                                                                                                                                                                                                                                                                                                    б. имеется указатель ср. рода </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>с!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> и отсутствует дефис или                                                                                                                                                                                                                                                                                                                    в. имеются указатель ср. рода </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>с</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> и указатель ср. рода с предшествующим дефисом </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-с</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>с</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>…</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-с</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>…).</t>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, и в ЗС имеется хотя бы 1 дефис.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Найти в БС строки с ЗС групп, идентификатор которых содержит </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.С </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>и не содержит символ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, и в ЗС имеется более 1 дефиса.</t>
     </r>
   </si>
 </sst>
@@ -6613,12 +7058,28 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6959,121 +7420,109 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -7081,117 +7530,140 @@
     <xf numFmtId="0" fontId="34" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7476,7 +7948,7 @@
   <dimension ref="A1:B93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A126" sqref="A126"/>
+      <selection activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7506,7 +7978,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7514,78 +7986,78 @@
         <v>10</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="84" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="87" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="27.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="85" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="29.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="86" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="27.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="77" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="29.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="76" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="73" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="78" t="s">
+      <c r="B13" s="83" t="s">
         <v>100</v>
       </c>
     </row>
@@ -7593,7 +8065,7 @@
       <c r="A14" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="78" t="s">
+      <c r="B14" s="75" t="s">
         <v>101</v>
       </c>
     </row>
@@ -7602,7 +8074,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -7617,88 +8089,88 @@
       <c r="A17" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="86" t="s">
+      <c r="B17" s="82" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="43" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="80" t="s">
-        <v>166</v>
+      <c r="A18" s="91" t="s">
+        <v>164</v>
       </c>
       <c r="B18" s="74" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B19" s="74" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="186.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="19" t="s">
-        <v>201</v>
+      <c r="A20" s="91" t="s">
+        <v>199</v>
       </c>
       <c r="B20" s="17" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="27" t="s">
-        <v>105</v>
+      <c r="B21" s="90" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="83" t="s">
-        <v>222</v>
+      <c r="B22" s="79" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="83" t="s">
-        <v>223</v>
+      <c r="B23" s="79" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="83" t="s">
-        <v>224</v>
+      <c r="B24" s="89" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="85" t="s">
-        <v>106</v>
+      <c r="B25" s="81" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="27" t="s">
-        <v>107</v>
+      <c r="B26" s="90" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="B27" s="79" t="s">
-        <v>217</v>
+        <v>143</v>
+      </c>
+      <c r="B27" s="76" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7706,7 +8178,7 @@
         <v>1</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7714,7 +8186,7 @@
         <v>17</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7722,7 +8194,7 @@
         <v>18</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7730,7 +8202,7 @@
         <v>19</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7738,7 +8210,7 @@
         <v>20</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7746,7 +8218,7 @@
         <v>21</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7754,7 +8226,7 @@
         <v>22</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7762,7 +8234,7 @@
         <v>23</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7770,7 +8242,7 @@
         <v>24</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -7778,7 +8250,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7786,7 +8258,7 @@
         <v>30</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7794,7 +8266,7 @@
         <v>32</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -7802,7 +8274,7 @@
         <v>31</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7810,7 +8282,7 @@
         <v>33</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7818,7 +8290,7 @@
         <v>34</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7826,15 +8298,15 @@
         <v>35</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="19" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7842,47 +8314,47 @@
         <v>43</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="81" t="s">
-        <v>221</v>
+      <c r="B46" s="77" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="81" t="s">
-        <v>220</v>
+      <c r="B47" s="77" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="81" t="s">
-        <v>218</v>
+      <c r="B48" s="77" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="84" t="s">
-        <v>115</v>
+      <c r="B49" s="80" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="B50" s="82" t="s">
-        <v>219</v>
+        <v>144</v>
+      </c>
+      <c r="B50" s="78" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7890,7 +8362,7 @@
         <v>2</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7898,7 +8370,7 @@
         <v>48</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7906,7 +8378,7 @@
         <v>49</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7914,7 +8386,7 @@
         <v>50</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7922,7 +8394,7 @@
         <v>51</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7930,7 +8402,7 @@
         <v>52</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7938,7 +8410,7 @@
         <v>53</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7946,7 +8418,7 @@
         <v>54</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7954,7 +8426,7 @@
         <v>55</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -7962,7 +8434,7 @@
         <v>56</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -7970,7 +8442,7 @@
         <v>57</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -7978,7 +8450,7 @@
         <v>58</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -7986,15 +8458,15 @@
         <v>59</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="25" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -8002,15 +8474,15 @@
         <v>60</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -8018,7 +8490,7 @@
         <v>3</v>
       </c>
       <c r="B67" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -8026,7 +8498,7 @@
         <v>61</v>
       </c>
       <c r="B68" s="27" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -8034,7 +8506,7 @@
         <v>63</v>
       </c>
       <c r="B69" s="27" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="30.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -8042,15 +8514,15 @@
         <v>62</v>
       </c>
       <c r="B70" s="29" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="30" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B71" s="31" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -8058,7 +8530,7 @@
         <v>64</v>
       </c>
       <c r="B72" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -8066,7 +8538,7 @@
         <v>65</v>
       </c>
       <c r="B73" s="31" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -8074,7 +8546,7 @@
         <v>66</v>
       </c>
       <c r="B74" s="31" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -8082,7 +8554,7 @@
         <v>67</v>
       </c>
       <c r="B75" s="34" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="76" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -8090,15 +8562,15 @@
         <v>4</v>
       </c>
       <c r="B76" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="77" spans="1:2" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="30" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B77" s="31" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="78" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -8106,7 +8578,7 @@
         <v>68</v>
       </c>
       <c r="B78" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="79" spans="1:2" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -8114,7 +8586,7 @@
         <v>69</v>
       </c>
       <c r="B79" s="31" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="80" spans="1:2" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -8122,7 +8594,7 @@
         <v>70</v>
       </c>
       <c r="B80" s="31" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="81" spans="1:2" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -8130,7 +8602,7 @@
         <v>71</v>
       </c>
       <c r="B81" s="34" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -8138,7 +8610,7 @@
         <v>72</v>
       </c>
       <c r="B82" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -8146,7 +8618,7 @@
         <v>73</v>
       </c>
       <c r="B83" s="35" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -8154,7 +8626,7 @@
         <v>79</v>
       </c>
       <c r="B84" s="35" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="85" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -8162,15 +8634,15 @@
         <v>74</v>
       </c>
       <c r="B85" s="37" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B86" s="38" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="87" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -8178,7 +8650,7 @@
         <v>75</v>
       </c>
       <c r="B87" s="36" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="88" spans="1:2" s="5" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -8186,15 +8658,15 @@
         <v>77</v>
       </c>
       <c r="B88" s="40" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="89" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="41" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B89" s="42" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="90" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -8202,7 +8674,7 @@
         <v>76</v>
       </c>
       <c r="B90" s="43" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="91" spans="1:2" s="8" customFormat="1" ht="160.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -8210,23 +8682,23 @@
         <v>78</v>
       </c>
       <c r="B91" s="44" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="92" spans="1:2" s="5" customFormat="1" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="45" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B92" s="46" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="93" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="47" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B93" s="48" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -8262,7 +8734,7 @@
         <v>80</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="6" customFormat="1" ht="89.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -8270,7 +8742,7 @@
         <v>81</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -8278,7 +8750,7 @@
         <v>82</v>
       </c>
       <c r="B4" s="53" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="7" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -8286,7 +8758,7 @@
         <v>83</v>
       </c>
       <c r="B5" s="53" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -8294,7 +8766,7 @@
         <v>84</v>
       </c>
       <c r="B6" s="53" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -8302,7 +8774,7 @@
         <v>85</v>
       </c>
       <c r="B7" s="53" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -8310,7 +8782,7 @@
         <v>86</v>
       </c>
       <c r="B8" s="53" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -8318,7 +8790,7 @@
         <v>87</v>
       </c>
       <c r="B9" s="53" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="7" customFormat="1" ht="116.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -8326,15 +8798,15 @@
         <v>88</v>
       </c>
       <c r="B10" s="53" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="6" customFormat="1" ht="203.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="54" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B11" s="55" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -8342,7 +8814,7 @@
         <v>89</v>
       </c>
       <c r="B12" s="56" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="7" customFormat="1" ht="129.6" x14ac:dyDescent="0.55000000000000004">
@@ -8350,7 +8822,7 @@
         <v>91</v>
       </c>
       <c r="B13" s="56" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="7" customFormat="1" ht="129.6" x14ac:dyDescent="0.55000000000000004">
@@ -8358,7 +8830,7 @@
         <v>92</v>
       </c>
       <c r="B14" s="56" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:2" s="6" customFormat="1" ht="44.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -8366,7 +8838,7 @@
         <v>95</v>
       </c>
       <c r="B15" s="58" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:2" s="7" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -8374,15 +8846,15 @@
         <v>96</v>
       </c>
       <c r="B16" s="68" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="7" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="66" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B17" s="59" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:2" s="7" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -8390,7 +8862,7 @@
         <v>90</v>
       </c>
       <c r="B18" s="70" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:2" s="7" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -8398,7 +8870,7 @@
         <v>93</v>
       </c>
       <c r="B19" s="71" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:2" s="7" customFormat="1" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -8406,23 +8878,23 @@
         <v>94</v>
       </c>
       <c r="B20" s="71" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:2" s="5" customFormat="1" ht="160.80000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="60" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B21" s="61" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:2" s="6" customFormat="1" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="62" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B22" s="63" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">

</xml_diff>